<commit_message>
Fixed the issue with double headers and messing with deep learning
</commit_message>
<xml_diff>
--- a/MLB/NRFI/NRFI-Tracker.xlsx
+++ b/MLB/NRFI/NRFI-Tracker.xlsx
@@ -28,6 +28,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-04-24" sheetId="20" state="visible" r:id="rId20"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-06-24" sheetId="21" state="visible" r:id="rId21"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-07-24" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-10-24" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -5053,6 +5054,187 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="21" t="inlineStr">
+        <is>
+          <t>Games</t>
+        </is>
+      </c>
+      <c r="B1" s="21" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('BOS', 'HOU')</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.738</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('ATL', 'COL')</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.731</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('NYM', 'SEA')</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.721</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('BAL', 'TB')</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.715</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('DET', 'SF')</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.698</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>('KC', 'STL')</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.674</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>('CHC', 'CWS')</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.522</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>('OAK', 'TOR')</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.522</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>('LAD', 'PIT')</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.501</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>('AZ', 'PHI')</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.478</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>('CLE', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>('LAA', 'WSH')</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.272</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>('NYY', 'TEX')</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>('CIN', 'MIL')</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>('MIA', 'SD')</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>